<commit_message>
Correccion Alex Preciarios en base a volumetrias
cambiar la forma de acualizar cantidad utilizad a acumulativa y cargarla
inicialmente en 0
</commit_message>
<xml_diff>
--- a/OSEF.ERP.APP/adjuntos/CR 0418 TONALA ZARAGOZA_FINAL.xlsx
+++ b/OSEF.ERP.APP/adjuntos/CR 0418 TONALA ZARAGOZA_FINAL.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="229">
   <si>
     <t>Concepto</t>
   </si>
@@ -733,6 +733,39 @@
   </si>
   <si>
     <t>Precio</t>
+  </si>
+  <si>
+    <t>B02</t>
+  </si>
+  <si>
+    <t>B03</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>C01</t>
+  </si>
+  <si>
+    <t>A0203</t>
+  </si>
+  <si>
+    <t>A03</t>
+  </si>
+  <si>
+    <t>A0301</t>
+  </si>
+  <si>
+    <t>A04</t>
+  </si>
+  <si>
+    <t>A0401</t>
+  </si>
+  <si>
+    <t>A0402</t>
+  </si>
+  <si>
+    <t>A0403</t>
   </si>
 </sst>
 </file>
@@ -1419,8 +1452,8 @@
   </sheetPr>
   <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2758,7 +2791,9 @@
       </c>
     </row>
     <row r="67" spans="1:7" s="5" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="20"/>
+      <c r="A67" s="20" t="s">
+        <v>222</v>
+      </c>
       <c r="B67" s="21" t="s">
         <v>95</v>
       </c>
@@ -2858,7 +2893,9 @@
       </c>
     </row>
     <row r="72" spans="1:7" s="29" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="35"/>
+      <c r="A72" s="35" t="s">
+        <v>223</v>
+      </c>
       <c r="B72" s="36" t="s">
         <v>100</v>
       </c>
@@ -2874,7 +2911,9 @@
       </c>
     </row>
     <row r="73" spans="1:7" s="5" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="20"/>
+      <c r="A73" s="20" t="s">
+        <v>224</v>
+      </c>
       <c r="B73" s="21" t="s">
         <v>137</v>
       </c>
@@ -2932,7 +2971,9 @@
       </c>
     </row>
     <row r="76" spans="1:7" s="29" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="35"/>
+      <c r="A76" s="35" t="s">
+        <v>225</v>
+      </c>
       <c r="B76" s="36" t="s">
         <v>102</v>
       </c>
@@ -2948,7 +2989,9 @@
       </c>
     </row>
     <row r="77" spans="1:7" s="5" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="20"/>
+      <c r="A77" s="20" t="s">
+        <v>226</v>
+      </c>
       <c r="B77" s="21" t="s">
         <v>103</v>
       </c>
@@ -2985,7 +3028,9 @@
       </c>
     </row>
     <row r="79" spans="1:7" s="5" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="20"/>
+      <c r="A79" s="20" t="s">
+        <v>227</v>
+      </c>
       <c r="B79" s="21" t="s">
         <v>104</v>
       </c>
@@ -3064,7 +3109,9 @@
       </c>
     </row>
     <row r="83" spans="1:7" s="5" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="20"/>
+      <c r="A83" s="20" t="s">
+        <v>228</v>
+      </c>
       <c r="B83" s="21" t="s">
         <v>107</v>
       </c>
@@ -3285,7 +3332,9 @@
       </c>
     </row>
     <row r="94" spans="1:7" s="5" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="41"/>
+      <c r="A94" s="41" t="s">
+        <v>218</v>
+      </c>
       <c r="B94" s="16" t="s">
         <v>118</v>
       </c>
@@ -3301,7 +3350,9 @@
       </c>
     </row>
     <row r="95" spans="1:7" s="5" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="41"/>
+      <c r="A95" s="41" t="s">
+        <v>219</v>
+      </c>
       <c r="B95" s="16" t="s">
         <v>119</v>
       </c>
@@ -3338,7 +3389,9 @@
       </c>
     </row>
     <row r="97" spans="1:7" s="5" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="10"/>
+      <c r="A97" s="10" t="s">
+        <v>220</v>
+      </c>
       <c r="B97" s="11" t="s">
         <v>121</v>
       </c>
@@ -3354,7 +3407,9 @@
       </c>
     </row>
     <row r="98" spans="1:7" s="5" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="15"/>
+      <c r="A98" s="15" t="s">
+        <v>221</v>
+      </c>
       <c r="B98" s="16" t="s">
         <v>113</v>
       </c>

</xml_diff>